<commit_message>
added stepsto read callouts
</commit_message>
<xml_diff>
--- a/src/main/resources/excel.xlsx
+++ b/src/main/resources/excel.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Locators" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Infotainment Callouts" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Safety" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
   <si>
     <t xml:space="preserve">className</t>
   </si>
@@ -49,7 +51,7 @@
     <t xml:space="preserve">Actual Font Colour</t>
   </si>
   <si>
-    <t xml:space="preserve">//*[@class='css-1ink1h8']</t>
+    <t xml:space="preserve">//*[@class='css-1pn4ll4']</t>
   </si>
   <si>
     <t xml:space="preserve">From $59,900 before savings and incentives with 0% APR*</t>
@@ -64,6 +66,9 @@
     <t xml:space="preserve">#101820</t>
   </si>
   <si>
+    <t xml:space="preserve">#000000</t>
+  </si>
+  <si>
     <t xml:space="preserve">//*[@class='css-3ycsxw']</t>
   </si>
   <si>
@@ -109,43 +114,16 @@
     <t xml:space="preserve">Free at home service and maintenance*</t>
   </si>
   <si>
-    <t>Element Not Found</t>
-  </si>
-  <si>
-    <t>From $59,900 before savings and incentives with 0% APR*</t>
-  </si>
-  <si>
-    <t>"Polestar Unica", "Helvetica Neue", Helvetica, Arial, sans-serif</t>
-  </si>
-  <si>
-    <t>16px</t>
-  </si>
-  <si>
-    <t>#000000</t>
-  </si>
-  <si>
-    <t>Lease from $599/month*</t>
-  </si>
-  <si>
-    <t>All-wheel drive</t>
-  </si>
-  <si>
-    <t>#101820</t>
-  </si>
-  <si>
-    <t>Dual electric motors</t>
-  </si>
-  <si>
-    <t>Largest charging network in U.S</t>
-  </si>
-  <si>
-    <t>233 miles on a single charge</t>
-  </si>
-  <si>
-    <t>0–62 mph in 4.47 sec</t>
-  </si>
-  <si>
-    <t>Free at home service and maintenance*</t>
+    <t xml:space="preserve">Callouts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free internet data for first 3 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+35% torsional stiffness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistive emergency braking</t>
   </si>
 </sst>
 </file>
@@ -155,7 +133,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -191,6 +169,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -234,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,6 +228,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -266,20 +254,20 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="24.29" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="51.0" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="53.3" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="17.71" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="19.57" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="0" width="19.57" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="17.71" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="0" width="19.57" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="53.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,7 +299,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -327,220 +315,220 @@
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" t="s">
-        <v>33</v>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4" t="s">
-        <v>36</v>
+      <c r="G4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" t="s">
-        <v>36</v>
+      <c r="F5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" t="s">
-        <v>36</v>
+      <c r="F6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" t="s">
-        <v>36</v>
+      <c r="F7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" t="s">
-        <v>36</v>
+      <c r="F8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" t="s">
-        <v>36</v>
+      <c r="F9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -552,4 +540,80 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.73"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>